<commit_message>
presentación y cambios en backlog
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anthonygregoryfloresramos/Docs/Duoc/Capstone/Documents/Fase 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A8510DC-CFFF-4241-BF94-6A3417325CF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CF2A48-ADB3-9745-94DA-3B06307AC776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product backlog normal" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="343">
   <si>
     <t>Identificador ID de la historia de usuario</t>
   </si>
@@ -1075,6 +1075,9 @@
   </si>
   <si>
     <t>Como cliente registrado, necesito ver la lista de servicios disponibles, para visualizar los servicios ofrecidos por DriveTail</t>
+  </si>
+  <si>
+    <t>Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -1663,7 +1666,7 @@
   </sheetPr>
   <dimension ref="B2:K38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -2133,9 +2136,9 @@
   </sheetPr>
   <dimension ref="A1:AA976"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N6" sqref="N6"/>
+      <selection pane="bottomLeft" activeCell="I90" sqref="B3:I90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3855,7 +3858,7 @@
         <v>20</v>
       </c>
       <c r="G41" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H41" s="15" t="s">
         <v>54</v>
@@ -3900,7 +3903,7 @@
         <v>43</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H42" s="18" t="s">
         <v>54</v>
@@ -3945,7 +3948,7 @@
         <v>20</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H43" s="18" t="s">
         <v>31</v>
@@ -3990,7 +3993,7 @@
         <v>20</v>
       </c>
       <c r="G44" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>31</v>
@@ -4035,7 +4038,7 @@
         <v>43</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H45" s="18" t="s">
         <v>54</v>
@@ -4080,7 +4083,7 @@
         <v>43</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H46" s="18" t="s">
         <v>54</v>
@@ -4125,7 +4128,7 @@
         <v>20</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>191</v>
+        <v>342</v>
       </c>
       <c r="H47" s="18" t="s">
         <v>54</v>
@@ -4571,8 +4574,8 @@
       <c r="F58" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G58" s="5" t="s">
-        <v>192</v>
+      <c r="G58" s="15" t="s">
+        <v>342</v>
       </c>
       <c r="H58" s="12" t="s">
         <v>54</v>
@@ -4616,8 +4619,8 @@
       <c r="F59" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G59" s="5" t="s">
-        <v>192</v>
+      <c r="G59" s="15" t="s">
+        <v>342</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>31</v>
@@ -4661,8 +4664,8 @@
       <c r="F60" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="G60" s="5" t="s">
-        <v>192</v>
+      <c r="G60" s="15" t="s">
+        <v>342</v>
       </c>
       <c r="H60" s="12" t="s">
         <v>31</v>
@@ -4736,7 +4739,7 @@
         <v>12</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H62" s="5" t="s">
         <v>31</v>
@@ -4781,7 +4784,7 @@
         <v>12</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H63" s="5" t="s">
         <v>31</v>
@@ -4826,7 +4829,7 @@
         <v>12</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H64" s="12" t="s">
         <v>31</v>
@@ -4871,7 +4874,7 @@
         <v>12</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H65" s="12" t="s">
         <v>31</v>
@@ -5109,7 +5112,7 @@
         <v>260</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>31</v>
@@ -5154,7 +5157,7 @@
         <v>260</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H72" s="5" t="s">
         <v>31</v>
@@ -5199,7 +5202,7 @@
         <v>260</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H73" s="12" t="s">
         <v>31</v>

</xml_diff>